<commit_message>
added time to timesheet, couple questions added to notes
</commit_message>
<xml_diff>
--- a/Stephen/TimesheetCS5010.xlsx
+++ b/Stephen/TimesheetCS5010.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Doyle\Documents\GitHub\CS5010_NotesEtc\Stephen\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="360" yWindow="75" windowWidth="27795" windowHeight="9270"/>
   </bookViews>
   <sheets>
     <sheet name="Timesheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
   <si>
     <t>Date</t>
   </si>
@@ -77,6 +82,9 @@
   </si>
   <si>
     <t>Total Time On Task Q1 (minutes)</t>
+  </si>
+  <si>
+    <t>Put together start of data definitions (world, mouse and key events)</t>
   </si>
 </sst>
 </file>
@@ -688,7 +696,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -723,7 +731,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -932,10 +940,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1043,83 +1051,126 @@
       </c>
     </row>
     <row r="6" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
+      <c r="A6" s="2">
+        <v>41688</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.37847222222222227</v>
+      </c>
+      <c r="E6" s="8">
+        <v>0</v>
+      </c>
+      <c r="G6" s="8">
+        <v>1</v>
+      </c>
+      <c r="I6" s="8">
+        <f>35</f>
+        <v>35</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="7" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="8" t="s">
+      <c r="A7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="9">
+        <f>A6</f>
+        <v>41688</v>
+      </c>
+      <c r="C7" s="10">
+        <f>D6</f>
+        <v>0.37847222222222227</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+    </row>
+    <row r="9" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="8" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+    <row r="10" spans="1:11" s="8" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="4">
-        <f>SUMIF(G2:G7,"1",I2:I7)</f>
-        <v>145</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="G10" s="4">
+        <f>SUMIF(G2:G9,"1",I2:I9)</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="4">
-        <f>SUMIF(G3:G7,"2",I3:I7)</f>
+      <c r="G11" s="4">
+        <f>SUMIF(G3:G9,"2",I3:I9)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="16.5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+    <row r="12" spans="1:11" ht="16.5" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="4">
-        <f>SUMIF(G3:G7,"3",I3:I7)</f>
+      <c r="G12" s="4">
+        <f>SUMIF(G3:G9,"3",I3:I9)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="16.5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+    <row r="13" spans="1:11" ht="16.5" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="4">
-        <f>SUMIF(G3:G7,"4",I3:I7)</f>
+      <c r="G13" s="4">
+        <f>SUMIF(G3:G9,"4",I3:I9)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="G13" s="3">
-        <f>G8/60</f>
-        <v>2.4166666666666665</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G14" s="3">
-        <f>G9/60</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="G15" s="3">
         <f>G10/60</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G16" s="3">
         <f>G11/60</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" s="3">
+        <f>G12/60</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G18" s="3">
+        <f>G13/60</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
worked on rendering nodes in a scene - got an initial cut working
</commit_message>
<xml_diff>
--- a/Stephen/TimesheetCS5010.xlsx
+++ b/Stephen/TimesheetCS5010.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Doyle\Documents\GitHub\CS5010_NotesEtc\Stephen\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="360" yWindow="75" windowWidth="27795" windowHeight="9270"/>
   </bookViews>
   <sheets>
     <sheet name="Timesheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="25">
   <si>
     <t>Date</t>
   </si>
@@ -85,6 +80,15 @@
   </si>
   <si>
     <t>Put together start of data definitions (world, mouse and key events)</t>
+  </si>
+  <si>
+    <t>Discussed tree of nodes with Steve</t>
+  </si>
+  <si>
+    <t>Got initial nodes-&gt;scene working (no lines etc)</t>
+  </si>
+  <si>
+    <t>Worked on world to scene</t>
   </si>
 </sst>
 </file>
@@ -696,7 +700,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -731,7 +735,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -940,10 +944,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="A4" sqref="A4:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1094,83 +1098,212 @@
       </c>
     </row>
     <row r="8" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
+      <c r="A8" s="2">
+        <v>41688</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="E8" s="8">
+        <v>0</v>
+      </c>
+      <c r="G8" s="8">
+        <v>1</v>
+      </c>
+      <c r="I8" s="8">
+        <f>60</f>
+        <v>60</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="9" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="8" t="s">
+      <c r="A9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="9">
+        <f>A8</f>
+        <v>41688</v>
+      </c>
+      <c r="C9" s="10">
+        <f>D8</f>
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>41688</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0.92708333333333337</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0.99375000000000002</v>
+      </c>
+      <c r="E10" s="8">
+        <v>0</v>
+      </c>
+      <c r="G10" s="8">
+        <v>1</v>
+      </c>
+      <c r="I10" s="8">
+        <f>45+51</f>
+        <v>96</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="9">
+        <f>A10</f>
+        <v>41688</v>
+      </c>
+      <c r="C11" s="10">
+        <f>D10</f>
+        <v>0.99375000000000002</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>41689</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0.36458333333333331</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0.39374999999999999</v>
+      </c>
+      <c r="E12" s="8">
+        <v>0</v>
+      </c>
+      <c r="G12" s="8">
+        <v>1</v>
+      </c>
+      <c r="I12" s="8">
+        <f>15+27</f>
+        <v>42</v>
+      </c>
+      <c r="K12" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="9">
+        <f>A12</f>
+        <v>41689</v>
+      </c>
+      <c r="C13" s="10">
+        <f>D12</f>
+        <v>0.39374999999999999</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+    </row>
+    <row r="15" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="8" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+    <row r="16" spans="1:11" s="8" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="4">
-        <f>SUMIF(G2:G9,"1",I2:I9)</f>
-        <v>180</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+      <c r="G16" s="4">
+        <f>SUMIF(G2:G15,"1",I2:I15)</f>
+        <v>378</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="4">
-        <f>SUMIF(G3:G9,"2",I3:I9)</f>
+      <c r="G17" s="4">
+        <f>SUMIF(G3:G15,"2",I3:I15)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="16.5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+    <row r="18" spans="1:7" ht="16.5" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G12" s="4">
-        <f>SUMIF(G3:G9,"3",I3:I9)</f>
+      <c r="G18" s="4">
+        <f>SUMIF(G3:G15,"3",I3:I15)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="16.5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+    <row r="19" spans="1:7" ht="16.5" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G13" s="4">
-        <f>SUMIF(G3:G9,"4",I3:I9)</f>
+      <c r="G19" s="4">
+        <f>SUMIF(G3:G15,"4",I3:I15)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G15" s="3">
-        <f>G10/60</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="G21" s="3">
+        <f>G16/60</f>
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G16" s="3">
-        <f>G11/60</f>
+      <c r="G22" s="3">
+        <f>G17/60</f>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G17" s="3">
-        <f>G12/60</f>
+      <c r="G23" s="3">
+        <f>G18/60</f>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G18" s="3">
-        <f>G13/60</f>
+      <c r="G24" s="3">
+        <f>G19/60</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
scenes*.rkt has lines now (but messy), added extras.rkt
</commit_message>
<xml_diff>
--- a/Stephen/TimesheetCS5010.xlsx
+++ b/Stephen/TimesheetCS5010.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="26">
   <si>
     <t>Date</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t>Worked on world to scene</t>
+  </si>
+  <si>
+    <t>Got lines for branches working</t>
   </si>
 </sst>
 </file>
@@ -944,10 +947,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD13"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1227,83 +1230,126 @@
       </c>
     </row>
     <row r="14" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
+      <c r="A14" s="2">
+        <v>41689</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0.72569444444444453</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0.74444444444444446</v>
+      </c>
+      <c r="E14" s="8">
+        <v>0</v>
+      </c>
+      <c r="G14" s="8">
+        <v>1</v>
+      </c>
+      <c r="I14" s="8">
+        <f>52-25</f>
+        <v>27</v>
+      </c>
+      <c r="K14" s="8" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="15" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="8" t="s">
+      <c r="A15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="9">
+        <f>A14</f>
+        <v>41689</v>
+      </c>
+      <c r="C15" s="10">
+        <f>D14</f>
+        <v>0.74444444444444446</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+    </row>
+    <row r="17" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="8" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+    <row r="18" spans="1:7" s="8" customFormat="1" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G16" s="4">
-        <f>SUMIF(G2:G15,"1",I2:I15)</f>
-        <v>378</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+      <c r="G18" s="4">
+        <f>SUMIF(G2:G17,"1",I2:I17)</f>
+        <v>405</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G17" s="4">
-        <f>SUMIF(G3:G15,"2",I3:I15)</f>
+      <c r="G19" s="4">
+        <f>SUMIF(G3:G17,"2",I3:I17)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="16.5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+    <row r="20" spans="1:7" ht="16.5" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G18" s="4">
-        <f>SUMIF(G3:G15,"3",I3:I15)</f>
+      <c r="G20" s="4">
+        <f>SUMIF(G3:G17,"3",I3:I17)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="16.5" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+    <row r="21" spans="1:7" ht="16.5" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G19" s="4">
-        <f>SUMIF(G3:G15,"4",I3:I15)</f>
+      <c r="G21" s="4">
+        <f>SUMIF(G3:G17,"4",I3:I17)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="G21" s="3">
-        <f>G16/60</f>
-        <v>6.3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G22" s="3">
-        <f>G17/60</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="G23" s="3">
         <f>G18/60</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>6.75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G24" s="3">
         <f>G19/60</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G25" s="3">
+        <f>G20/60</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G26" s="3">
+        <f>G21/60</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>